<commit_message>
[Main board] First complete schematic
</commit_message>
<xml_diff>
--- a/doc/main_board_bom.xlsx
+++ b/doc/main_board_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nagragrp-my.sharepoint.com/personal/jean-pierre_maitre_nagra_com/Documents/Documents/Privé/Electronique/TheMagicKeys/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="256" documentId="11_F25DC773A252ABDACC10482F61DE5A9A5ADE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA5D27F9-1AA1-47CC-AE73-1D3B2C1ECCAD}"/>
+  <xr:revisionPtr revIDLastSave="259" documentId="11_F25DC773A252ABDACC10482F61DE5A9A5ADE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1DCB3A2-9FA3-4737-8063-813A35A169F8}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31830" yWindow="1470" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,7 +471,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +604,7 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>23</v>

</xml_diff>